<commit_message>
CDS Test cases Study Facet and Many to Many test cases.
</commit_message>
<xml_diff>
--- a/InputFiles/CDS/TC11_CDS_Filter_PHSAccession-phs002529.xlsx
+++ b/InputFiles/CDS/TC11_CDS_Filter_PHSAccession-phs002529.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation 0707\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation\Sowjanya0320\Commons_Automation\InputFiles\CDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAF31D4-F73F-4073-B0CF-5B2B949AD3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F79A310-055A-4003-B17E-11B01D5069AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{013465C6-4E4F-447A-BFCF-6610D055375C}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{013465C6-4E4F-447A-BFCF-6610D055375C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,114 +56,450 @@
     <t>ParticipantsTab</t>
   </si>
   <si>
-    <t>SamplesTab</t>
-  </si>
-  <si>
-    <t>FilesTab</t>
-  </si>
-  <si>
-    <t>TC11_CDS_Filter_PHSAccession-phs002529_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC11_CDS_Filter_PHSAccession-phs002529_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>CALL{
-    MATCH (p:participant)--&gt;(s:study)
-    OPTIONAL MATCH (samp:sample)--&gt;(p)
+    <t>WITH {
+    phs_accession: "phs002529",
+    subject_ids: [],
+    experimental_strategies: [],
+    genders: [],
+    sample_tumor_statuses: [],
+    file_types: [],
+    library_strategies: [],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+MATCH (s:study {phs_accession: inputs.phs_accession})
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH inputs, na, s, count(distinct p) AS num_p
+WHERE
+    (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+    (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, s, count(distinct samp) AS num_samp
+WHERE
+    (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+    (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+MATCH (s)&lt;--(p:participant)
+WITH inputs, na, p, {
+participant_id: coalesce(p.participant_id, ""),
+study_name: coalesce(s.study_name, ""),
+accession: coalesce(s.phs_accession, ""),
+gender: coalesce(p.gender, "")
+} AS data
+WHERE
+    (size(inputs.subject_ids) = 0 OR p.participant_id IN inputs.subject_ids) AND
+    (size(inputs.genders) = 0 OR p.gender IN inputs.genders)
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+WITH inputs, na, p, apoc.map.merge(data, {
+samples: coalesce(apoc.text.join(apoc.coll.sort(collect(distinct samp.sample_id)), ", "), "")
+}) AS data,
+COLLECT(DISTINCT samp.sample_tumor_status) AS sample_tumor_statuses
+WHERE
+    (size(inputs.sample_tumor_statuses) = 0 OR size(apoc.coll.intersection(inputs.sample_tumor_statuses, sample_tumor_statuses)) &gt; 0)
+OPTIONAL MATCH (p)&lt;--(:sample)&lt;--(f:file)
+WITH inputs, na, p, data,
+COLLECT(DISTINCT f.file_type) AS file_types,
+apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+WHERE
+    (size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+    (size(inputs.file_types) = 0 OR size(apoc.coll.intersection(inputs.file_types, file_types)) &gt; 0)
+OPTIONAL MATCH (p)&lt;--(:sample)&lt;--(:file)&lt;--(g:genomic_info)
+WITH inputs, na, p, data,
+COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+COLLECT(DISTINCT g.library_source) AS library_source,
+COLLECT(DISTINCT g.library_selection) AS library_selection,
+COLLECT(DISTINCT g.library_layout) AS library_layout,
+COLLECT(DISTINCT g.platform) AS platform,
+COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+WHERE
+    (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+    (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND
+    (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+    (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+    (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+    (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+    (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+WITH inputs, na, p, data,
+COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+WHERE
+    (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
+RETURN
+data.participant_id AS `Participant ID`,
+data.study_name AS `Study Name`,
+data.accession AS `Accession`,
+data.gender AS `Gender`,
+data.samples AS `Samples`
+ORDER BY `Participant ID`
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002529",
+    subject_ids: [],
+    experimental_strategies: [],
+    genders: [],
+    sample_tumor_statuses: [],
+    file_types: [],
+    library_strategies: [],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+CALL{
+    WITH inputs, na
+    MATCH (s:study {phs_accession: inputs.phs_accession})
+    OPTIONAL MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, s, count(distinct p) AS num_p
+    WHERE
+        (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+        (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+    OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, s, count(distinct samp) AS num_samp
+    WHERE
+        (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+        (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+    MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, p
+    WHERE
+        (size(inputs.subject_ids) = 0 OR p.participant_id IN inputs.subject_ids) AND
+        (size(inputs.genders) = 0 OR p.gender IN inputs.genders)
+    OPTIONAL MATCH (p)&lt;--(samp:sample)
+    WITH inputs, na, p, samp
+    WHERE
+        (size(inputs.sample_tumor_statuses) = 0 OR (samp is not null AND coalesce(samp.sample_tumor_status, na) IN inputs.sample_tumor_statuses))
     OPTIONAL MATCH (samp)&lt;--(f:file)
+    UNWIND coalesce(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}"), na) AS experimental_strategies
+    WITH inputs, na, p, f, experimental_strategies
+    WHERE
+        (size(inputs.experimental_strategies) = 0 OR (f is not null AND experimental_strategies IN inputs.experimental_strategies)) AND
+        (size(inputs.file_types) = 0 OR (f is not null AND coalesce(f.file_type, na) IN inputs.file_types))
     OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+    WITH inputs, na, p, g
+    WHERE
+        (size(inputs.library_strategies) = 0 OR (g is not null AND coalesce(g.library_strategy , na) IN inputs.library_strategies)) AND
+        (size(inputs.library_sources) = 0 OR (g is not null AND coalesce(g.library_source , na) IN inputs.library_sources)) AND
+        (size(inputs.library_selections) = 0 OR (g is not null AND coalesce(g.library_selection , na) IN inputs.library_selections)) AND
+        (size(inputs.library_layouts) = 0 OR (g is not null AND coalesce(g.library_layout , na) IN inputs.library_layouts)) AND
+        (size(inputs.platforms) = 0 OR (g is not null AND coalesce(g.platform , na) IN inputs.platforms)) AND
+        (size(inputs.instrument_models) = 0 OR (g is not null AND coalesce(g.instrument_model , na) IN inputs.instrument_models)) AND
+        (size(inputs.reference_genome_assemblies) = 0 OR (g is not null AND coalesce(g.reference_genome_assembly , na) IN inputs.reference_genome_assemblies))
     OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-    WITH s, p, samp, f, g, diag
-    WHERE s.phs_accession in ["phs002529"]
-    RETURN 
+    WITH inputs, na, p, diag
+    WHERE
+        (size(inputs.primary_diagnoses) = 0 OR (diag is not null AND coalesce(diag.primary_diagnosis, na) IN inputs.primary_diagnoses))
+    RETURN
         count(distinct p) AS num_participants
-}
-WITH num_participants
+    }
+WITH inputs, na, num_participants
 CALL {
-    MATCH (samp:sample)--&gt;(p:participant)--&gt;(s)
+    WITH inputs, na
+    MATCH (s:study {phs_accession: inputs.phs_accession})
+    OPTIONAL MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, s, count(distinct p) AS num_p
+    WHERE
+        (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+        (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+    OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, s, count(distinct samp) AS num_samp
+    WHERE
+        (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+        (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+    MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, samp
+    WHERE
+        (size(inputs.sample_tumor_statuses) = 0 OR coalesce(samp.sample_tumor_status, na) IN inputs.sample_tumor_statuses)
+    OPTIONAL MATCH (samp)--&gt;(p:participant)
+    WITH inputs, na, samp, p
+    WHERE
+        (size(inputs.subject_ids) = 0 OR (p is not null AND p.participant_id IN inputs.subject_ids)) AND
+        (size(inputs.genders) = 0 OR (p is not null AND p.gender IN inputs.genders))
     OPTIONAL MATCH (samp)&lt;--(f:file)
-    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+    UNWIND coalesce(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}"), na) AS experimental_strategies
+    WITH inputs, na, samp, f, experimental_strategies
+    WHERE
+        (size(inputs.experimental_strategies) = 0 OR (f is not null AND experimental_strategies IN inputs.experimental_strategies)) AND
+        (size(inputs.file_types) = 0 OR (f is not null AND coalesce(f.file_type, na) IN inputs.file_types))
     OPTIONAL MATCH (f)&lt;--(g:genomic_info)
-    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-    WITH s, p, samp, f, g, diag
-    WHERE s.phs_accession in ["phs002529"]
-    RETURN 
+    WITH inputs, na, samp, g
+    WHERE
+        (size(inputs.library_strategies) = 0 OR (g is not null AND coalesce(g.library_strategy , na) IN inputs.library_strategies)) AND
+        (size(inputs.library_sources) = 0 OR (g is not null AND coalesce(g.library_source , na) IN inputs.library_sources)) AND
+        (size(inputs.library_selections) = 0 OR (g is not null AND coalesce(g.library_selection , na) IN inputs.library_selections)) AND
+        (size(inputs.library_layouts) = 0 OR (g is not null AND coalesce(g.library_layout , na) IN inputs.library_layouts)) AND
+        (size(inputs.platforms) = 0 OR (g is not null AND coalesce(g.platform , na) IN inputs.platforms)) AND
+        (size(inputs.instrument_models) = 0 OR (g is not null AND coalesce(g.instrument_model , na) IN inputs.instrument_models)) AND
+        (size(inputs.reference_genome_assemblies) = 0 OR (g is not null AND coalesce(g.reference_genome_assembly , na) IN inputs.reference_genome_assemblies))
+    OPTIONAL MATCH (samp)--&gt;(:participant)&lt;--(diag:diagnosis)
+    WITH inputs, na, samp, diag
+    WHERE
+        (size(inputs.primary_diagnoses) = 0 OR (diag is not null AND coalesce(diag.primary_diagnosis, na) IN inputs.primary_diagnoses))
+    RETURN
         count(distinct samp) AS num_samples
 }
-WITH num_participants, num_samples
+WITH inputs, na, num_participants, num_samples
 CALL {
-    MATCH (f:file)--&gt;(s:study)
+    WITH inputs, na
+    MATCH (s:study {phs_accession: inputs.phs_accession})
+    OPTIONAL MATCH (s)&lt;--(p:participant)
+    WITH inputs, na, s, count(distinct p) AS num_p
+    WHERE
+        (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+        (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+    OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+    WITH inputs, na, s, count(distinct samp) AS num_samp
+    WHERE
+        (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+        (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+    MATCH (s)&lt;--(f:file)
+    UNWIND coalesce(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}"), na) AS experimental_strategies
+    WITH inputs, na, f, experimental_strategies
+    WHERE
+        (size(inputs.experimental_strategies) = 0 OR experimental_strategies IN inputs.experimental_strategies) AND
+        (size(inputs.file_types) = 0 OR coalesce(f.file_type, na) IN inputs.file_types)
+    OPTIONAL MATCH (f)--&gt;(samp:sample)
+    WITH inputs, na, f, samp
+    WHERE
+        (size(inputs.sample_tumor_statuses) = 0 OR (samp is not null AND coalesce(samp.sample_tumor_status, na) IN inputs.sample_tumor_statuses))
+    OPTIONAL MATCH (samp)--&gt;(p:participant)
+    WITH inputs, na, f, p
+    WHERE
+        (size(inputs.subject_ids) = 0 OR (p is not null AND p.participant_id IN inputs.subject_ids)) AND
+        (size(inputs.genders) = 0 OR (p is not null AND p.gender IN inputs.genders))
     OPTIONAL MATCH (f)&lt;--(g:genomic_info)
-    OPTIONAL MATCH (samp:sample)&lt;--(f)
-    OPTIONAL MATCH (p:participant)&lt;--(samp)
-    OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-    WITH s, p, samp, f, g, diag
-    WHERE s.phs_accession in ["phs002529"]
-    RETURN 
-        count(distinct s) AS num_studies,
+    WITH inputs, na, f, g
+    WHERE
+        (size(inputs.library_strategies) = 0 OR (g is not null AND coalesce(g.library_strategy , na) IN inputs.library_strategies)) AND
+        (size(inputs.library_sources) = 0 OR (g is not null AND coalesce(g.library_source , na) IN inputs.library_sources)) AND
+        (size(inputs.library_selections) = 0 OR (g is not null AND coalesce(g.library_selection , na) IN inputs.library_selections)) AND
+        (size(inputs.library_layouts) = 0 OR (g is not null AND coalesce(g.library_layout , na) IN inputs.library_layouts)) AND
+        (size(inputs.platforms) = 0 OR (g is not null AND coalesce(g.platform , na) IN inputs.platforms)) AND
+        (size(inputs.instrument_models) = 0 OR (g is not null AND coalesce(g.instrument_model , na) IN inputs.instrument_models)) AND
+        (size(inputs.reference_genome_assemblies) = 0 OR (g is not null AND coalesce(g.reference_genome_assembly , na) IN inputs.reference_genome_assemblies))
+    OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(:participant)&lt;--(diag:diagnosis)
+    WITH inputs, na, f, diag
+    WHERE
+        (size(inputs.primary_diagnoses) = 0 OR coalesce(diag.primary_diagnosis, na) IN inputs.primary_diagnoses)
+    RETURN
         count(distinct f) AS num_files
 }
-RETURN 
-    num_studies AS Studies,
+RETURN
+    1 AS Studies,
     num_participants AS Participants,
     num_samples AS Samples,
     num_files AS `Files`</t>
   </si>
   <si>
-    <t>MATCH (f:file)--&gt;(s:study)
-OPTIONAL MATCH (samp:sample)&lt;--(f)
+    <t>TC11_CDS_Filter_PHSAccession-phs002529_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC11_CDS_Filter_PHSAccession-phs002529_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002529",
+    subject_ids: [],
+    experimental_strategies: [],
+    genders: [],
+    sample_tumor_statuses: [],
+    file_types: [],
+    library_strategies: [],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+MATCH (s:study {phs_accession: inputs.phs_accession})
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH inputs, na, s, count(distinct p) AS num_p
+WHERE
+    (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+    (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, s, count(distinct samp) AS num_samp
+WHERE
+    (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+    (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, samp, {
+sample_id: samp.sample_id,
+study_name: s.study_name,
+accession: s.phs_accession,
+tumor: samp.sample_tumor_status,
+analyte_type: samp.sample_type
+} AS data
+WHERE
+    (size(inputs.sample_tumor_statuses) = 0 OR samp.sample_tumor_status IN inputs.sample_tumor_statuses)
 OPTIONAL MATCH (samp)--&gt;(p:participant)
+WITH inputs, na, samp,
+apoc.map.merge(data, {
+participant_id: p.participant_id
+}) AS data,
+COLLECT(DISTINCT p.participant_id) AS participant_id,
+COLLECT(DISTINCT p.gender) AS gender
+WHERE
+    (size(inputs.subject_ids) = 0 OR size(apoc.coll.intersection(inputs.participant_id, participant_id)) &gt; 0) AND
+    (size(inputs.genders) = 0 OR size(apoc.coll.intersection(inputs.gender, gender)) &gt; 0)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+WITH inputs, na, samp, data,
+COLLECT(DISTINCT f.file_types) AS file_types,
+apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+WHERE
+(size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+    (size(inputs.file_types) = 0 OR size(apoc.coll.intersection(inputs.file_types, file_types)) &gt; 0)
+OPTIONAL MATCH (samp)&lt;--(:file)&lt;--(g:genomic_info)
+WITH inputs, na, samp, data,
+COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+COLLECT(DISTINCT g.library_source) AS library_source,
+COLLECT(DISTINCT g.library_selection) AS library_selection,
+COLLECT(DISTINCT g.library_layout) AS library_layout,
+COLLECT(DISTINCT g.platform) AS platform,
+COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+WHERE
+    (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+    (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND
+    (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+    (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+    (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+    (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+    (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+OPTIONAL MATCH (samp)--&gt;(:participant)&lt;--(diag:diagnosis)
+WITH inputs, na, samp, data,
+COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+WHERE
+    (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnosis, primary_diagnosis)) &gt; 0)
+RETURN
+data.sample_id AS `Sample ID`,
+data.participant_id AS `Participant ID`,
+data.study_name AS `Study Name`,
+data.accession AS `Accession`,
+data.tumor AS `Tumor`,
+data.analyte_type AS `Analyte Type`
+ORDER BY `Sample ID`
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>WITH {
+    phs_accession: "phs002529",
+    subject_ids: [],
+    experimental_strategies: [],
+    genders: [],
+    sample_tumor_statuses: [],
+    file_types: [],
+    library_strategies: [],
+    library_sources: [],
+    library_selections: [],
+    library_layouts: [],
+    platforms: [],
+    instrument_models: [],
+    reference_genome_assemblies: [],
+    primary_diagnoses: [],
+    num_study_samples_min: 0,
+    num_study_samples_max: 0,
+    num_study_participants_max: 0,
+    num_study_participants_min: 0
+} AS inputs, "Not specified in data" AS na
+MATCH (s:study {phs_accession: inputs.phs_accession})
+OPTIONAL MATCH (s)&lt;--(p:participant)
+WITH inputs, na, s, count(distinct p) AS num_p
+WHERE
+    (inputs.num_study_participants_min = 0 OR num_p &gt;= inputs.num_study_participants_min) AND
+    (inputs.num_study_participants_max = 0 OR num_p &lt;= inputs.num_study_participants_max)
+OPTIONAL MATCH (s)&lt;--(:participant)&lt;--(samp:sample)
+WITH inputs, na, s, count(distinct samp) AS num_samp
+WHERE
+    (inputs.num_study_samples_min = 0 OR num_samp &gt;= inputs.num_study_samples_min) AND
+    (inputs.num_study_participants_max = 0 OR num_samp &lt;= inputs.num_study_participants_max)
+MATCH (s)&lt;--(f:file)
+WITH inputs, na, f, {
+file_name: coalesce(f.file_name, ""),
+file_type: coalesce(f.file_type, ""),
+study_name: coalesce(s.study_name, ""),
+accession: coalesce(s.phs_accession, "")
+} AS data,
+apoc.coll.toSet(apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}")) AS experimental_strategies
+WHERE
+(size(inputs.experimental_strategies) = 0 OR size(apoc.coll.intersection(inputs.experimental_strategies, experimental_strategies)) &gt; 0) AND
+    (size(inputs.file_types) = 0 OR f.file_type IN inputs.file_types)
+OPTIONAL MATCH (f)--&gt;(samp)
+WITH inputs, na, f, apoc.map.merge(data, {
+sample_id: coalesce(apoc.text.join(apoc.coll.sort(collect(distinct samp.sample_id)), ", "), "")
+}) AS data,
+COLLECT(DISTINCT samp.sample_tumor_status) AS sample_tumor_status
+WHERE
+(size(inputs.sample_tumor_statuses) = 0 OR size(apoc.coll.intersection(inputs.sample_tumor_statuses, sample_tumor_status)) &gt; 0)
+OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(p:participant)
+WITH inputs, na, f,
+apoc.map.merge(data, {
+participant_id: coalesce(apoc.text.join(collect(distinct p.participant_id), ", "), "")
+}) AS data,
+COLLECT(DISTINCT p.participant_id) AS participant_id,
+COLLECT(DISTINCT p.gender) AS gender
+WHERE
+    (size(inputs.subject_ids) = 0 OR size(apoc.coll.intersection(inputs.participant_id, participant_id)) &gt; 0) AND
+    (size(inputs.genders) = 0 OR size(apoc.coll.intersection(inputs.gender, gender)) &gt; 0)
 OPTIONAL MATCH (f)&lt;--(g:genomic_info)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-WITH s, p, samp, f, g, diag
-WHERE s.phs_accession in ["phs002529"]
-WITH DISTINCT f, s, p, samp
+WITH inputs, na, f, data,
+COLLECT(DISTINCT g.library_strategy) AS library_strategy,
+COLLECT(DISTINCT g.library_source) AS library_source,
+COLLECT(DISTINCT g.library_selection) AS library_selection,
+COLLECT(DISTINCT g.library_layout) AS library_layout,
+COLLECT(DISTINCT g.platform) AS platform,
+COLLECT(DISTINCT g.instrument_model) AS instrument_models,
+COLLECT(DISTINCT g.reference_genome_assembly) AS reference_genome_assembly
+WHERE
+    (size(inputs.library_strategies) = 0 OR size(apoc.coll.intersection(inputs.library_strategies, library_strategy)) &gt; 0) AND
+    (size(inputs.library_sources) = 0 OR size(apoc.coll.intersection(inputs.library_sources, library_source)) &gt; 0) AND
+    (size(inputs.library_selections) = 0 OR size(apoc.coll.intersection(inputs.library_selections, library_selection)) &gt; 0) AND
+    (size(inputs.library_layouts) = 0 OR size(apoc.coll.intersection(inputs.library_layouts, library_layout)) &gt; 0) AND
+    (size(inputs.platforms) = 0 OR size(apoc.coll.intersection(inputs.platforms, platform)) &gt; 0) AND
+    (size(inputs.instrument_models) = 0 OR size(apoc.coll.intersection(inputs.instrument_models, instrument_models)) &gt; 0) AND
+    (size(inputs.reference_genome_assemblies) = 0 OR size(apoc.coll.intersection(inputs.reference_genome_assemblies, reference_genome_assembly)) &gt; 0)
+OPTIONAL MATCH (f)--&gt;(:sample)--&gt;(:participant)&lt;--(diag:diagnosis)
+WITH inputs, na, f, data,
+COLLECT(DISTINCT diag.primary_diagnosis) AS primary_diagnosis
+WHERE
+    (size(inputs.primary_diagnoses) = 0 OR size(apoc.coll.intersection(inputs.primary_diagnoses, primary_diagnosis)) &gt; 0)
 RETURN
-    coalesce(f.file_name, '') as `File Name`,
-    coalesce(s.study_name,'') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.participant_id, '') as `Participant ID`,
-    coalesce(samp.sample_id, '') as `Sample ID`,
-    coalesce(f.file_type, '') as `File Type`
-ORDER BY f.file_name limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (samp:sample)--&gt;(p:participant)--&gt;(s:study)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-OPTIONAL MATCH (f)&lt;--(g:genomic_info)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-WITH s, p, samp, f, g, diag
-WHERE s.phs_accession in ["phs002529"]
-WITH DISTINCT s, p, samp
-RETURN
-    coalesce(samp.sample_id, '') as `Sample ID`,
-    coalesce(p.participant_id,'') as `Participant ID`,
-    coalesce(s.study_name, '') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(samp.sample_tumor_status,'') as `Tumor`,
-    coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER BY samp.sample_id limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (p:participant)--&gt;(s:study)
-OPTIONAL MATCH (samp:sample)--&gt;(p)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-OPTIONAL MATCH (f)&lt;--(g:genomic_info)
-WITH s, p, samp, f, g, diag
-WHERE s.phs_accession in ["phs002529"]
-WITH p
-OPTIONAL MATCH (p)--&gt;(s:study)
-OPTIONAL MATCH (samp:sample)--&gt;(p)
-WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
-RETURN 
-coalesce(p.participant_id,'') as `Participant ID`,
-coalesce(s.study_name, '') as `Study Name`,
-coalesce(s.phs_accession,'') as `Accession`,
-coalesce(p.gender,'') as `Gender`,
-coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY p.participant_id limit 100</t>
+data.file_name AS `File Name`,
+data.study_name AS `Study Name`,
+data.accession AS `Accession`,
+data.participant_id AS `Participant Id`,
+data.sample_id AS `Sample Id`,
+data.file_type AS `File Type`
+ORDER BY `File Name`
+LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -179,11 +515,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -208,10 +543,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,19 +865,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3821241-AD5E-4858-88C9-B7B397D860C9}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.7109375" customWidth="1"/>
-    <col min="4" max="4" width="70.28515625" customWidth="1"/>
-    <col min="5" max="5" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.69140625" customWidth="1"/>
+    <col min="4" max="4" width="70.3046875" customWidth="1"/>
+    <col min="5" max="5" width="63.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,15 +894,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -576,15 +911,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -593,15 +928,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -610,14 +945,301 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3A4EFB22810614D921FE8B7E7DAEFA8" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="244521d1350ace1b48ec0d9e0c7b13f4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5901cbfa-22a5-460e-a18e-d2e48de81980" xmlns:ns3="c68fef7c-f1b9-468c-b56b-b081b4f51826" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c1cb0894ef4fd2c5225ebadab417008d" ns2:_="" ns3:_="">
+    <xsd:import namespace="5901cbfa-22a5-460e-a18e-d2e48de81980"/>
+    <xsd:import namespace="c68fef7c-f1b9-468c-b56b-b081b4f51826"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5901cbfa-22a5-460e-a18e-d2e48de81980" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="8ce9f98e-9ad5-43de-b59a-72d7e946aae0" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="21" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c68fef7c-f1b9-468c-b56b-b081b4f51826" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{d077d19b-969d-4cda-adcf-2a29173dd2a8}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="c68fef7c-f1b9-468c-b56b-b081b4f51826">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5901cbfa-22a5-460e-a18e-d2e48de81980">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c68fef7c-f1b9-468c-b56b-b081b4f51826" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60393082-7270-4909-921D-7900E1128587}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D1836F9-537F-41A9-96CA-D7F7666AE17C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5901cbfa-22a5-460e-a18e-d2e48de81980"/>
+    <ds:schemaRef ds:uri="c68fef7c-f1b9-468c-b56b-b081b4f51826"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F54448A0-9A7E-495D-A245-5F6DFFE3C271}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5901cbfa-22a5-460e-a18e-d2e48de81980"/>
+    <ds:schemaRef ds:uri="c68fef7c-f1b9-468c-b56b-b081b4f51826"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>